<commit_message>
Added Greeting and Name Detector
</commit_message>
<xml_diff>
--- a/Final Project/chatdata.xlsx
+++ b/Final Project/chatdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DA6D05-A554-8E43-9541-A2F33570F99D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6877FBE2-8267-7343-92B8-E37B50C96972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="860" windowWidth="25440" windowHeight="14120" xr2:uid="{D35DFF8D-3322-0B40-B50D-0AABE77BDEFF}"/>
+    <workbookView xWindow="3360" yWindow="500" windowWidth="25440" windowHeight="14120" xr2:uid="{D35DFF8D-3322-0B40-B50D-0AABE77BDEFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
   <si>
     <t>Group</t>
   </si>
@@ -154,6 +154,288 @@
   </si>
   <si>
     <t>Hello nice to meet you</t>
+  </si>
+  <si>
+    <t>Nice to meet you</t>
+  </si>
+  <si>
+    <t>Glad to meet you</t>
+  </si>
+  <si>
+    <t>Doing fine</t>
+  </si>
+  <si>
+    <t>how is your day?</t>
+  </si>
+  <si>
+    <t>I am nice to meet you</t>
+  </si>
+  <si>
+    <t>Good morning nice to meet you</t>
+  </si>
+  <si>
+    <t>Good evening glad to meet you</t>
+  </si>
+  <si>
+    <t>Good afternoon nice to meet you</t>
+  </si>
+  <si>
+    <t>Hey hey</t>
+  </si>
+  <si>
+    <t>Hi Hi</t>
+  </si>
+  <si>
+    <t>Hiii</t>
+  </si>
+  <si>
+    <t>Helloooo</t>
+  </si>
+  <si>
+    <t>Hi are you ok</t>
+  </si>
+  <si>
+    <t>Great to meet you</t>
+  </si>
+  <si>
+    <t>heyyyy</t>
+  </si>
+  <si>
+    <t>Good to meet you</t>
+  </si>
+  <si>
+    <t>Hi I'm Nice to meet you</t>
+  </si>
+  <si>
+    <t>Hello I am glad to meet you</t>
+  </si>
+  <si>
+    <t>I'm nice to meet you</t>
+  </si>
+  <si>
+    <t>My name is nice to meet you</t>
+  </si>
+  <si>
+    <t>My name is glad to meet you</t>
+  </si>
+  <si>
+    <t>Ho Ho</t>
+  </si>
+  <si>
+    <t>Hello Hello</t>
+  </si>
+  <si>
+    <t>Hi Good Day</t>
+  </si>
+  <si>
+    <t>Hello Good Day</t>
+  </si>
+  <si>
+    <t>Good Noon</t>
+  </si>
+  <si>
+    <t>It's pleasure to meet you</t>
+  </si>
+  <si>
+    <t>Good Morning I'm Nice to meet you</t>
+  </si>
+  <si>
+    <t>How are the things with you</t>
+  </si>
+  <si>
+    <t>G'day</t>
+  </si>
+  <si>
+    <t>Good Day</t>
+  </si>
+  <si>
+    <t>It's good to see you</t>
+  </si>
+  <si>
+    <t>It is good to see you</t>
+  </si>
+  <si>
+    <t>Hey there</t>
+  </si>
+  <si>
+    <t>How's it's going</t>
+  </si>
+  <si>
+    <t>Yo!</t>
+  </si>
+  <si>
+    <t>Hi I'm . I would like to know about your services</t>
+  </si>
+  <si>
+    <t>Hello I am . I need to know about services</t>
+  </si>
+  <si>
+    <t>I need to know about your saloon services</t>
+  </si>
+  <si>
+    <t>Hello Good Mornning. I am . I need to know about your serives</t>
+  </si>
+  <si>
+    <t>Hi! Good Evening. What are services your saloon provide?</t>
+  </si>
+  <si>
+    <t>What are the available services</t>
+  </si>
+  <si>
+    <t>What can I get from you?</t>
+  </si>
+  <si>
+    <t>Good Morning. I would like to know about services</t>
+  </si>
+  <si>
+    <t>I'm . I would like to know your saloon services</t>
+  </si>
+  <si>
+    <t>Morning! What can I get from you?</t>
+  </si>
+  <si>
+    <t>My name is . I like to know available services</t>
+  </si>
+  <si>
+    <t>I'm what services do you offer</t>
+  </si>
+  <si>
+    <t>Hi! what services could I get from your saloon</t>
+  </si>
+  <si>
+    <t>Any available services</t>
+  </si>
+  <si>
+    <t>Hey what services are available?</t>
+  </si>
+  <si>
+    <t>Howdy! I need to know about your services</t>
+  </si>
+  <si>
+    <t>Afternoon I need to know about your services</t>
+  </si>
+  <si>
+    <t>I would like to know about services</t>
+  </si>
+  <si>
+    <t>I like to know available services</t>
+  </si>
+  <si>
+    <t>I like to know about services</t>
+  </si>
+  <si>
+    <t>What services would I get?</t>
+  </si>
+  <si>
+    <t>What could I get frok your saloon</t>
+  </si>
+  <si>
+    <t>Good Morning! What are the available services?</t>
+  </si>
+  <si>
+    <t>Good Evening! I need to know about services?</t>
+  </si>
+  <si>
+    <t>Well, Could you please tell me about services?</t>
+  </si>
+  <si>
+    <t>Hey, Could you plese provide information about services?</t>
+  </si>
+  <si>
+    <t>Hi, I need to know about saloon services</t>
+  </si>
+  <si>
+    <t>What are the services?</t>
+  </si>
+  <si>
+    <t>Availble services please</t>
+  </si>
+  <si>
+    <t>We need to know about services</t>
+  </si>
+  <si>
+    <t>We would like to know about available services</t>
+  </si>
+  <si>
+    <t>How are you? I need to know about available services</t>
+  </si>
+  <si>
+    <t>How you are doing? By the way I need to know about services</t>
+  </si>
+  <si>
+    <t>Hope you are doing well. I would like to know about saloon</t>
+  </si>
+  <si>
+    <t>I would like to know about saloon</t>
+  </si>
+  <si>
+    <t>I need to know about saloon prices</t>
+  </si>
+  <si>
+    <t>Hey! I would like know about saloon prices</t>
+  </si>
+  <si>
+    <t>Hellooo</t>
+  </si>
+  <si>
+    <t>Hello hope that everythin going fine</t>
+  </si>
+  <si>
+    <t>Good Good Morning</t>
+  </si>
+  <si>
+    <t>Goooood Morning</t>
+  </si>
+  <si>
+    <t>hello hi</t>
+  </si>
+  <si>
+    <t>hi hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hi hello I'm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hello hi my name is </t>
+  </si>
+  <si>
+    <t>Morning My name is</t>
+  </si>
+  <si>
+    <t>Evening I'm .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Afternoon I am </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello good morning. I am </t>
+  </si>
+  <si>
+    <t>Hi Good evening. My name is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello Morning. I'm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello! Good Morning. How are you? I am </t>
+  </si>
+  <si>
+    <t>Hi Evening. I am . Nice to meet you</t>
+  </si>
+  <si>
+    <t>Howdy. I am . How are you?</t>
+  </si>
+  <si>
+    <t>Good Morning. What can I get from your saloon</t>
+  </si>
+  <si>
+    <t>good afternoon. I would like to know about saloon prices</t>
+  </si>
+  <si>
+    <t>Good Morning. I am . Could you please provide saloon services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">good afternoon. My name is . I would like to know about </t>
   </si>
 </sst>
 </file>
@@ -511,15 +793,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B284F1-251B-6F44-B7B1-B1D020E6424A}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="58.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="5" width="10.83203125" style="2"/>
     <col min="6" max="6" width="27.33203125" style="2" customWidth="1"/>
@@ -846,6 +1128,762 @@
         <v>1</v>
       </c>
     </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B70" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B79" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B81" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B83" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B87" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B89" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B100" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B101" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B102" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B103" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B105" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B106" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B107" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B108" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B109" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B110" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B111" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B112" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B113" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B114" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B115" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B116" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B117" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B118" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B119" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B120" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B121" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B122" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B123" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B124" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B125" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B126" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B127" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B128" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B129" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B130" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B131" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B132" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Saloon services groups
</commit_message>
<xml_diff>
--- a/Final Project/chatdata.xlsx
+++ b/Final Project/chatdata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Chathuranga/Desktop/Masters Lecture Docs/Text Mining 732A92 /Labs/Text Mining Labs/Final Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6877FBE2-8267-7343-92B8-E37B50C96972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBDB8E2-A302-3C47-B3D6-DF575B7C6002}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="500" windowWidth="25440" windowHeight="14120" xr2:uid="{D35DFF8D-3322-0B40-B50D-0AABE77BDEFF}"/>
+    <workbookView xWindow="160" yWindow="640" windowWidth="25440" windowHeight="14120" xr2:uid="{D35DFF8D-3322-0B40-B50D-0AABE77BDEFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="174">
   <si>
     <t>Group</t>
   </si>
@@ -45,24 +45,6 @@
     <t xml:space="preserve">Hi! </t>
   </si>
   <si>
-    <t>Good Morning!</t>
-  </si>
-  <si>
-    <t>Good Evening!</t>
-  </si>
-  <si>
-    <t>Good Afternoon!</t>
-  </si>
-  <si>
-    <t>Morning!</t>
-  </si>
-  <si>
-    <t>Hey!</t>
-  </si>
-  <si>
-    <t>Hey How are you?</t>
-  </si>
-  <si>
     <t>how are you?</t>
   </si>
   <si>
@@ -72,18 +54,12 @@
     <t>Hola</t>
   </si>
   <si>
-    <t>Hello</t>
-  </si>
-  <si>
     <t>How are you?</t>
   </si>
   <si>
     <t>Hi how are you?</t>
   </si>
   <si>
-    <t>Hello how are you?</t>
-  </si>
-  <si>
     <t>Hola how are you?</t>
   </si>
   <si>
@@ -93,30 +69,9 @@
     <t>Hope you are doing well?</t>
   </si>
   <si>
-    <t>Hello hope you are doing well?</t>
-  </si>
-  <si>
-    <t>Evening</t>
-  </si>
-  <si>
-    <t>Hi Good Evening</t>
-  </si>
-  <si>
-    <t>Hello Good Evening</t>
-  </si>
-  <si>
-    <t>Hi Good Afternoon</t>
-  </si>
-  <si>
-    <t>Hello Good Afternoon</t>
-  </si>
-  <si>
     <t>Hi Good Morning</t>
   </si>
   <si>
-    <t>Hello Good Morning</t>
-  </si>
-  <si>
     <t>How do you do?</t>
   </si>
   <si>
@@ -132,30 +87,6 @@
     <t>How you doing</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello, I'm </t>
-  </si>
-  <si>
-    <t>My name is</t>
-  </si>
-  <si>
-    <t>I am</t>
-  </si>
-  <si>
-    <t>Hi  here</t>
-  </si>
-  <si>
-    <t>Hi My name is</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hi! I'm </t>
-  </si>
-  <si>
-    <t>This is</t>
-  </si>
-  <si>
-    <t>Hello nice to meet you</t>
-  </si>
-  <si>
     <t>Nice to meet you</t>
   </si>
   <si>
@@ -168,18 +99,6 @@
     <t>how is your day?</t>
   </si>
   <si>
-    <t>I am nice to meet you</t>
-  </si>
-  <si>
-    <t>Good morning nice to meet you</t>
-  </si>
-  <si>
-    <t>Good evening glad to meet you</t>
-  </si>
-  <si>
-    <t>Good afternoon nice to meet you</t>
-  </si>
-  <si>
     <t>Hey hey</t>
   </si>
   <si>
@@ -204,36 +123,15 @@
     <t>Good to meet you</t>
   </si>
   <si>
-    <t>Hi I'm Nice to meet you</t>
-  </si>
-  <si>
-    <t>Hello I am glad to meet you</t>
-  </si>
-  <si>
     <t>I'm nice to meet you</t>
   </si>
   <si>
-    <t>My name is nice to meet you</t>
-  </si>
-  <si>
-    <t>My name is glad to meet you</t>
-  </si>
-  <si>
     <t>Ho Ho</t>
   </si>
   <si>
-    <t>Hello Hello</t>
-  </si>
-  <si>
     <t>Hi Good Day</t>
   </si>
   <si>
-    <t>Hello Good Day</t>
-  </si>
-  <si>
-    <t>Good Noon</t>
-  </si>
-  <si>
     <t>It's pleasure to meet you</t>
   </si>
   <si>
@@ -255,30 +153,15 @@
     <t>It is good to see you</t>
   </si>
   <si>
-    <t>Hey there</t>
-  </si>
-  <si>
     <t>How's it's going</t>
   </si>
   <si>
     <t>Yo!</t>
   </si>
   <si>
-    <t>Hi I'm . I would like to know about your services</t>
-  </si>
-  <si>
-    <t>Hello I am . I need to know about services</t>
-  </si>
-  <si>
     <t>I need to know about your saloon services</t>
   </si>
   <si>
-    <t>Hello Good Mornning. I am . I need to know about your serives</t>
-  </si>
-  <si>
-    <t>Hi! Good Evening. What are services your saloon provide?</t>
-  </si>
-  <si>
     <t>What are the available services</t>
   </si>
   <si>
@@ -288,15 +171,6 @@
     <t>Good Morning. I would like to know about services</t>
   </si>
   <si>
-    <t>I'm . I would like to know your saloon services</t>
-  </si>
-  <si>
-    <t>Morning! What can I get from you?</t>
-  </si>
-  <si>
-    <t>My name is . I like to know available services</t>
-  </si>
-  <si>
     <t>I'm what services do you offer</t>
   </si>
   <si>
@@ -312,9 +186,6 @@
     <t>Howdy! I need to know about your services</t>
   </si>
   <si>
-    <t>Afternoon I need to know about your services</t>
-  </si>
-  <si>
     <t>I would like to know about services</t>
   </si>
   <si>
@@ -333,15 +204,9 @@
     <t>Good Morning! What are the available services?</t>
   </si>
   <si>
-    <t>Good Evening! I need to know about services?</t>
-  </si>
-  <si>
     <t>Well, Could you please tell me about services?</t>
   </si>
   <si>
-    <t>Hey, Could you plese provide information about services?</t>
-  </si>
-  <si>
     <t>Hi, I need to know about saloon services</t>
   </si>
   <si>
@@ -372,70 +237,325 @@
     <t>I need to know about saloon prices</t>
   </si>
   <si>
-    <t>Hey! I would like know about saloon prices</t>
-  </si>
-  <si>
     <t>Hellooo</t>
   </si>
   <si>
-    <t>Hello hope that everythin going fine</t>
-  </si>
-  <si>
-    <t>Good Good Morning</t>
-  </si>
-  <si>
-    <t>Goooood Morning</t>
-  </si>
-  <si>
-    <t>hello hi</t>
-  </si>
-  <si>
-    <t>hi hello</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hi hello I'm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hello hi my name is </t>
-  </si>
-  <si>
-    <t>Morning My name is</t>
-  </si>
-  <si>
-    <t>Evening I'm .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good Afternoon I am </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello good morning. I am </t>
-  </si>
-  <si>
-    <t>Hi Good evening. My name is</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello Morning. I'm </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello! Good Morning. How are you? I am </t>
-  </si>
-  <si>
-    <t>Hi Evening. I am . Nice to meet you</t>
-  </si>
-  <si>
-    <t>Howdy. I am . How are you?</t>
-  </si>
-  <si>
     <t>Good Morning. What can I get from your saloon</t>
   </si>
   <si>
-    <t>good afternoon. I would like to know about saloon prices</t>
-  </si>
-  <si>
-    <t>Good Morning. I am . Could you please provide saloon services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">good afternoon. My name is . I would like to know about </t>
+    <t>Hi! I'm username</t>
+  </si>
+  <si>
+    <t>Hi My name is username</t>
+  </si>
+  <si>
+    <t>My name is username</t>
+  </si>
+  <si>
+    <t>This is username</t>
+  </si>
+  <si>
+    <t>I am username</t>
+  </si>
+  <si>
+    <t>Hi username  here</t>
+  </si>
+  <si>
+    <t>I am username .nice to meet you</t>
+  </si>
+  <si>
+    <t>Hi I'm username Nice to meet you</t>
+  </si>
+  <si>
+    <t>My name is username nice to meet you</t>
+  </si>
+  <si>
+    <t>My name is username glad to meet you</t>
+  </si>
+  <si>
+    <t>Hi I'm username. I would like to know about your services</t>
+  </si>
+  <si>
+    <t>I'm username. I would like to know your saloon services</t>
+  </si>
+  <si>
+    <t>My name is username. I like to know available services</t>
+  </si>
+  <si>
+    <t>Howdy. I am username . How are you?</t>
+  </si>
+  <si>
+    <t>Good Morning. I am username. Could you please provide saloon services</t>
+  </si>
+  <si>
+    <t>I'm doing fine. How about you</t>
+  </si>
+  <si>
+    <t>How about you</t>
+  </si>
+  <si>
+    <t>Hope you are fine</t>
+  </si>
+  <si>
+    <t>Hi, I'm username</t>
+  </si>
+  <si>
+    <t>Hi!</t>
+  </si>
+  <si>
+    <t>Hi How are you?</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Hi hope you are doing well?</t>
+  </si>
+  <si>
+    <t>Hi nice to meet you</t>
+  </si>
+  <si>
+    <t>Hi I am username .glad to meet you</t>
+  </si>
+  <si>
+    <t>Hi I am username. I need to know about services</t>
+  </si>
+  <si>
+    <t>Hi, Could you plese provide information about services?</t>
+  </si>
+  <si>
+    <t>Hi! I would like know about saloon prices</t>
+  </si>
+  <si>
+    <t>Hi hope that everythin going fine</t>
+  </si>
+  <si>
+    <t>Hi Hi I'm username</t>
+  </si>
+  <si>
+    <t>Hi Hi my name is username</t>
+  </si>
+  <si>
+    <t>Good Morning</t>
+  </si>
+  <si>
+    <t>Good Morning nice to meet you</t>
+  </si>
+  <si>
+    <t>Good Morning glad to meet you</t>
+  </si>
+  <si>
+    <t>Hi Good Morning. I am username. I need to know about your serives</t>
+  </si>
+  <si>
+    <t>Hi! Good Morning. What are services your saloon provide?</t>
+  </si>
+  <si>
+    <t>Good Morning! What can I get from you?</t>
+  </si>
+  <si>
+    <t>Good Morning I need to know about your services</t>
+  </si>
+  <si>
+    <t>Good Morning! I need to know about services?</t>
+  </si>
+  <si>
+    <t>Goooood Good Morning</t>
+  </si>
+  <si>
+    <t>Good Morning My name is username</t>
+  </si>
+  <si>
+    <t>Good Morning I'm username.</t>
+  </si>
+  <si>
+    <t>Good Morning I am username</t>
+  </si>
+  <si>
+    <t>Hi Good Morning. I am username</t>
+  </si>
+  <si>
+    <t>Hi Good Morning. My name is username</t>
+  </si>
+  <si>
+    <t>Hi Good Morning. I'm username</t>
+  </si>
+  <si>
+    <t>Hi! Good Morning. How are you? I am username</t>
+  </si>
+  <si>
+    <t>Hi Good Morning. I am username. Nice to meet you</t>
+  </si>
+  <si>
+    <t>Good Morning. I would like to know about saloon prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good Morning. My name is  username. I would like to know about </t>
+  </si>
+  <si>
+    <t>Morning. How are you?</t>
+  </si>
+  <si>
+    <t>Hi Morning. I am username. How are you?</t>
+  </si>
+  <si>
+    <t>Morning I am username. Are you fine?</t>
+  </si>
+  <si>
+    <t>Are you doing fine?</t>
+  </si>
+  <si>
+    <t>Hi hi are you fine?</t>
+  </si>
+  <si>
+    <t>Are you ok?</t>
+  </si>
+  <si>
+    <t>you okay?</t>
+  </si>
+  <si>
+    <t>Morning . Are you ok?</t>
+  </si>
+  <si>
+    <t>Hi. Are you okay?</t>
+  </si>
+  <si>
+    <t>Hello Morning Are you doing fine?</t>
+  </si>
+  <si>
+    <t>Hi Morning. My name is username, How are you?</t>
+  </si>
+  <si>
+    <t>Hi Nice to meet you are you doing fine?</t>
+  </si>
+  <si>
+    <t>Hey Are you doing great</t>
+  </si>
+  <si>
+    <t>Good Morning I would like to know your services</t>
+  </si>
+  <si>
+    <t>Hey Good Morning I need to know about your services</t>
+  </si>
+  <si>
+    <t>Hey hello What are the services I could get from you</t>
+  </si>
+  <si>
+    <t>What are the service availble on your saloon</t>
+  </si>
+  <si>
+    <t>Good Morning could you please tell me the services</t>
+  </si>
+  <si>
+    <t>Could you please provide saloon services</t>
+  </si>
+  <si>
+    <t>Could you please tell me the saloon prices</t>
+  </si>
+  <si>
+    <t>Can you please give me further information about saloon services</t>
+  </si>
+  <si>
+    <t>Can I know about the saloon services</t>
+  </si>
+  <si>
+    <t>I am willing to know saloon service</t>
+  </si>
+  <si>
+    <t>Hey I want to know saloon services</t>
+  </si>
+  <si>
+    <t>Good Morning I want to know available saloon services</t>
+  </si>
+  <si>
+    <t>Hey Morning I need to know about availble saloon services</t>
+  </si>
+  <si>
+    <t>Hey I would like to know available services</t>
+  </si>
+  <si>
+    <t>Morning I need saloon services information</t>
+  </si>
+  <si>
+    <t>Hi I need to know about saloon prices</t>
+  </si>
+  <si>
+    <t>What services are you providing?</t>
+  </si>
+  <si>
+    <t>Morning I would like to know the services</t>
+  </si>
+  <si>
+    <t>Morning Could you tell me the saloon services</t>
+  </si>
+  <si>
+    <t>Hey Are you okay</t>
+  </si>
+  <si>
+    <t>Hey are you ok</t>
+  </si>
+  <si>
+    <t>Morning you doing fine</t>
+  </si>
+  <si>
+    <t>I am doing fine. How are you</t>
+  </si>
+  <si>
+    <t>Morning I am doing fine. How are you</t>
+  </si>
+  <si>
+    <t>Hey how you doing</t>
+  </si>
+  <si>
+    <t>Hey whats up?</t>
+  </si>
+  <si>
+    <t>hey whatz up</t>
+  </si>
+  <si>
+    <t>hey are you fine</t>
+  </si>
+  <si>
+    <t>hey I'm fine thank you. How about you</t>
+  </si>
+  <si>
+    <t>Morning. I am feeling fine. How about you</t>
+  </si>
+  <si>
+    <t>Hey. I'm doing fine. Hope that you doing fine too</t>
+  </si>
+  <si>
+    <t>I am doing great. How are you?</t>
+  </si>
+  <si>
+    <t>I'm fine. So how about you</t>
+  </si>
+  <si>
+    <t>Hey how are you?</t>
+  </si>
+  <si>
+    <t>Hi how is with you</t>
+  </si>
+  <si>
+    <t>Morning. How about you</t>
+  </si>
+  <si>
+    <t>you doing okay</t>
+  </si>
+  <si>
+    <t>hope that you are ok too</t>
+  </si>
+  <si>
+    <t>hope that you are okay too</t>
+  </si>
+  <si>
+    <t>I'm fine. How are you</t>
+  </si>
+  <si>
+    <t>I'm good. How about you</t>
+  </si>
+  <si>
+    <t>I am fine. How about you</t>
   </si>
 </sst>
 </file>
@@ -793,10 +913,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B284F1-251B-6F44-B7B1-B1D020E6424A}">
-  <dimension ref="A1:B136"/>
+  <dimension ref="A1:B181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,7 +946,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -834,7 +954,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -842,7 +962,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -850,55 +970,55 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="B8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -906,23 +1026,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -930,7 +1050,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -938,47 +1058,47 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1">
         <v>2</v>
@@ -986,7 +1106,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
@@ -994,15 +1114,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B25" s="1">
         <v>2</v>
@@ -1010,7 +1130,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B26" s="1">
         <v>2</v>
@@ -1018,15 +1138,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B28" s="1">
         <v>2</v>
@@ -1034,71 +1154,71 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>22</v>
+        <v>92</v>
       </c>
       <c r="B30" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B32" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="B35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>28</v>
+        <v>101</v>
       </c>
       <c r="B36" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>29</v>
+        <v>102</v>
       </c>
       <c r="B37" s="1">
         <v>1</v>
@@ -1106,23 +1226,23 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="B38" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -1130,7 +1250,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -1138,7 +1258,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -1146,7 +1266,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B43" s="1">
         <v>2</v>
@@ -1154,15 +1274,15 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B44" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B45" s="1">
         <v>1</v>
@@ -1170,31 +1290,31 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B46" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="B47" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="B48" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1">
         <v>1</v>
@@ -1202,7 +1322,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -1210,7 +1330,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="B51" s="1">
         <v>1</v>
@@ -1218,7 +1338,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B52" s="1">
         <v>1</v>
@@ -1226,23 +1346,23 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="B54" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>54</v>
+        <v>100</v>
       </c>
       <c r="B55" s="1">
         <v>1</v>
@@ -1250,23 +1370,23 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="B56" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="B57" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B58" s="1">
         <v>2</v>
@@ -1274,31 +1394,31 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B59" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B60" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="B61" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="B62" s="1">
         <v>1</v>
@@ -1306,7 +1426,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="B63" s="1">
         <v>1</v>
@@ -1314,7 +1434,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="B64" s="1">
         <v>1</v>
@@ -1322,23 +1442,23 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="B65" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B66" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B67" s="1">
         <v>3</v>
@@ -1346,31 +1466,31 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B68" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="B69" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="B70" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="B71" s="1">
         <v>3</v>
@@ -1378,7 +1498,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="B72" s="1">
         <v>3</v>
@@ -1386,351 +1506,351 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B73" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B74" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B75" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="B76" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B77" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="B78" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B79" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="B80" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B81" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="B82" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="B83" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="B84" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="B85" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="B86" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="B87" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="B88" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="B89" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="B90" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="B91" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B92" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="B93" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="B94" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="B95" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
       <c r="B96" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="B97" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B98" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>96</v>
+        <v>63</v>
       </c>
       <c r="B99" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="B100" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="B101" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="B102" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B103" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B104" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B105" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B106" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B107" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="B108" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B109" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B110" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B111" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B112" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B113" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B114" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B115" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B116" s="1">
         <v>1</v>
@@ -1738,7 +1858,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B117" s="1">
         <v>2</v>
@@ -1746,103 +1866,103 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B118" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="B119" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>117</v>
+        <v>68</v>
       </c>
       <c r="B120" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B121" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="B122" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B123" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="B124" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="B125" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B126" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B127" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B128" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B129" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B130" s="1">
         <v>2</v>
@@ -1850,7 +1970,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B131" s="1">
         <v>2</v>
@@ -1858,7 +1978,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B132" s="1">
         <v>2</v>
@@ -1866,22 +1986,394 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="B133" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
+      </c>
+      <c r="B134" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
+      </c>
+      <c r="B135" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B136" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B137" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B138" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B139" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B140" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
         <v>133</v>
+      </c>
+      <c r="B141" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B142" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B143" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B144" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B145" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B146" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B147" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B148" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B149" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B150" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B151" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B152" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B153" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B154" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B155" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B156" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B157" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B158" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B159" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B160" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B161" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B162" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B163" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B164" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B165" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B166" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B167" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B168" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B169" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B170" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B171" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B172" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B173" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B174" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B175" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B176" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B177" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B178" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B179" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B180" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B181" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>